<commit_message>
git config --global user.email "you@example.com"
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\framework-pom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DC014692-9BC4-450B-92F5-0D25E87B2578}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A35A05D-F271-4CAE-9E97-9CD5FA230B58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E978D1C6-F70F-40D2-BF1D-B4A0F1A826DC}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Front End</t>
   </si>
@@ -55,6 +55,39 @@
   </si>
   <si>
     <t>SP and Table migration</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>Letter Sent</t>
+  </si>
+  <si>
+    <t>Exclusion</t>
+  </si>
+  <si>
+    <t>Exception</t>
+  </si>
+  <si>
+    <t>Special Request</t>
+  </si>
+  <si>
+    <t>Letter Search</t>
+  </si>
+  <si>
+    <t>Files</t>
+  </si>
+  <si>
+    <t>Upload</t>
+  </si>
+  <si>
+    <t>Download</t>
+  </si>
+  <si>
+    <t>Maintenance</t>
+  </si>
+  <si>
+    <t>Delete Letter</t>
   </si>
 </sst>
 </file>
@@ -86,7 +119,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -94,18 +127,80 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -421,81 +516,253 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99CBE502-23B4-4F92-A911-7E62AC948FF0}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2" t="s">
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="2"/>
-    </row>
-    <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K1" s="3"/>
+    </row>
+    <row r="2" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="I1:J1"/>
+  <mergeCells count="5">
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="B8:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>